<commit_message>
Adicionei uma pasta com o projeto do pupeetter
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemos\Desktop\Projetos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemos\Desktop\Projetos\Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3B8955-1B21-4D5B-AFC4-685C1B2FEBB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9CF1FB-78F5-44FE-B513-ED22470D440B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,7 +629,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1255,11 +1255,11 @@
         <v>24</v>
       </c>
       <c r="C24" s="7">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="P24" s="4">
         <f>SUM(C24:O24)</f>
-        <v>504</v>
+        <v>512</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1269,9 +1269,7 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="7">
-        <v>331.21</v>
-      </c>
+      <c r="C26" s="7"/>
       <c r="D26" s="3">
         <v>331.21</v>
       </c>
@@ -1295,7 +1293,7 @@
       </c>
       <c r="P26" s="4">
         <f>SUM(C26:O26)</f>
-        <v>2649.68</v>
+        <v>2318.4699999999998</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1305,9 +1303,7 @@
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="7">
-        <v>677.2</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="3">
         <v>30.65</v>
       </c>
@@ -1319,7 +1315,7 @@
       <c r="J27" s="3"/>
       <c r="P27" s="4">
         <f>SUM(C27:O27)</f>
-        <v>707.85</v>
+        <v>30.65</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1329,9 +1325,7 @@
       <c r="B28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="7">
-        <v>150</v>
-      </c>
+      <c r="C28" s="7"/>
       <c r="D28" s="3">
         <v>150</v>
       </c>
@@ -1345,7 +1339,7 @@
       <c r="J28" s="3"/>
       <c r="P28" s="4">
         <f>SUM(C28:O28)</f>
-        <v>450</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -1355,9 +1349,7 @@
       <c r="B29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="7">
-        <v>86.66</v>
-      </c>
+      <c r="C29" s="7"/>
       <c r="D29" s="3">
         <v>86.66</v>
       </c>
@@ -1378,9 +1370,7 @@
       <c r="B30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="7">
-        <v>420</v>
-      </c>
+      <c r="C30" s="7"/>
       <c r="D30" s="3">
         <v>420</v>
       </c>
@@ -1459,7 +1449,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="5">
         <f t="shared" ref="C35:N35" si="3">SUM(C13:C33)</f>
-        <v>3735.7699999999995</v>
+        <v>2078.6999999999998</v>
       </c>
       <c r="D35" s="5">
         <f t="shared" si="3"/>
@@ -1507,13 +1497,13 @@
       </c>
       <c r="P35" s="12">
         <f>SUM(P13:P33)</f>
-        <v>10798.74</v>
+        <v>9648.33</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C37" s="12">
         <f t="shared" ref="C37:N37" si="4">C11+C35</f>
-        <v>4660.6499999999996</v>
+        <v>3003.58</v>
       </c>
       <c r="D37" s="12">
         <f t="shared" si="4"/>
@@ -1620,60 +1610,58 @@
         <v>36</v>
       </c>
       <c r="C40" s="3">
-        <v>1735.22</v>
+        <v>541.44000000000005</v>
       </c>
       <c r="D40" s="3">
         <f t="shared" ref="D40:N40" si="5">C47</f>
-        <v>104.57000000000062</v>
+        <v>37.860000000000127</v>
       </c>
       <c r="E40" s="3">
         <f t="shared" si="5"/>
-        <v>923.48000000000047</v>
+        <v>856.76999999999953</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="5"/>
-        <v>40.720000000000255</v>
+        <v>-25.990000000000691</v>
       </c>
       <c r="G40" s="3">
         <f t="shared" si="5"/>
-        <v>2502.1100000000006</v>
+        <v>2435.3999999999996</v>
       </c>
       <c r="H40" s="3">
         <f t="shared" si="5"/>
-        <v>2491.5400000000009</v>
+        <v>2424.83</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="5"/>
-        <v>2695.7600000000011</v>
+        <v>2629.05</v>
       </c>
       <c r="J40" s="3">
         <f t="shared" si="5"/>
-        <v>2899.9800000000014</v>
+        <v>2833.2700000000004</v>
       </c>
       <c r="K40" s="3">
         <f t="shared" si="5"/>
-        <v>3726.7600000000011</v>
+        <v>3660.05</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" si="5"/>
-        <v>4884.7500000000009</v>
+        <v>4818.04</v>
       </c>
       <c r="M40" s="3">
         <f t="shared" si="5"/>
-        <v>6042.7400000000007</v>
+        <v>5976.03</v>
       </c>
       <c r="N40" s="3">
         <f t="shared" si="5"/>
-        <v>7200.7300000000014</v>
+        <v>7134.0199999999986</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="3">
-        <v>330</v>
-      </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1687,16 +1675,14 @@
       <c r="N41" s="3"/>
       <c r="P41" s="4">
         <f>P35+P11</f>
-        <v>26185.730000000003</v>
+        <v>25035.32</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="3">
-        <v>200</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="3">
         <v>200</v>
       </c>
@@ -1740,51 +1726,51 @@
       </c>
       <c r="C45" s="7">
         <f t="shared" ref="C45:N45" si="6">SUM(C39:C43)</f>
-        <v>4765.22</v>
+        <v>3041.44</v>
       </c>
       <c r="D45" s="7">
         <f t="shared" si="6"/>
-        <v>6037.1900000000005</v>
+        <v>5970.48</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="6"/>
-        <v>3423.4800000000005</v>
+        <v>3356.7699999999995</v>
       </c>
       <c r="F45" s="7">
         <f t="shared" si="6"/>
-        <v>5540.72</v>
+        <v>5474.0099999999993</v>
       </c>
       <c r="G45" s="7">
         <f t="shared" si="6"/>
-        <v>5002.1100000000006</v>
+        <v>4935.3999999999996</v>
       </c>
       <c r="H45" s="7">
         <f t="shared" si="6"/>
-        <v>4991.5400000000009</v>
+        <v>4924.83</v>
       </c>
       <c r="I45" s="7">
         <f t="shared" si="6"/>
-        <v>5195.7600000000011</v>
+        <v>5129.05</v>
       </c>
       <c r="J45" s="7">
         <f t="shared" si="6"/>
-        <v>5399.9800000000014</v>
+        <v>5333.27</v>
       </c>
       <c r="K45" s="7">
         <f t="shared" si="6"/>
-        <v>6226.7600000000011</v>
+        <v>6160.05</v>
       </c>
       <c r="L45" s="7">
         <f t="shared" si="6"/>
-        <v>7384.7500000000009</v>
+        <v>7318.04</v>
       </c>
       <c r="M45" s="7">
         <f t="shared" si="6"/>
-        <v>8542.7400000000016</v>
+        <v>8476.0299999999988</v>
       </c>
       <c r="N45" s="7">
         <f t="shared" si="6"/>
-        <v>12500.730000000001</v>
+        <v>12434.019999999999</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -1793,51 +1779,51 @@
       </c>
       <c r="C47" s="5">
         <f t="shared" ref="C47:N47" si="7">C45-C37</f>
-        <v>104.57000000000062</v>
+        <v>37.860000000000127</v>
       </c>
       <c r="D47" s="5">
         <f t="shared" si="7"/>
-        <v>923.48000000000047</v>
+        <v>856.76999999999953</v>
       </c>
       <c r="E47" s="5">
         <f t="shared" si="7"/>
-        <v>40.720000000000255</v>
+        <v>-25.990000000000691</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="7"/>
-        <v>2502.1100000000006</v>
+        <v>2435.3999999999996</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="7"/>
-        <v>2491.5400000000009</v>
+        <v>2424.83</v>
       </c>
       <c r="H47" s="5">
         <f t="shared" si="7"/>
-        <v>2695.7600000000011</v>
+        <v>2629.05</v>
       </c>
       <c r="I47" s="5">
         <f t="shared" si="7"/>
-        <v>2899.9800000000014</v>
+        <v>2833.2700000000004</v>
       </c>
       <c r="J47" s="5">
         <f t="shared" si="7"/>
-        <v>3726.7600000000011</v>
+        <v>3660.05</v>
       </c>
       <c r="K47" s="5">
         <f t="shared" si="7"/>
-        <v>4884.7500000000009</v>
+        <v>4818.04</v>
       </c>
       <c r="L47" s="5">
         <f t="shared" si="7"/>
-        <v>6042.7400000000007</v>
+        <v>5976.03</v>
       </c>
       <c r="M47" s="5">
         <f t="shared" si="7"/>
-        <v>7200.7300000000014</v>
+        <v>7134.0199999999986</v>
       </c>
       <c r="N47" s="5">
         <f t="shared" si="7"/>
-        <v>11158.720000000001</v>
+        <v>11092.009999999998</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -1847,26 +1833,15 @@
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C51" s="3">
-        <v>577.20000000000005</v>
-      </c>
-      <c r="D51" s="3">
-        <v>828</v>
-      </c>
-      <c r="E51" s="3">
-        <v>257</v>
-      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="3">
-        <f>SUM(C51:E51)</f>
-        <v>1662.2</v>
-      </c>
-      <c r="H51" s="3">
-        <v>200</v>
-      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
       <c r="J51" s="5">
         <f>G51+H51</f>
-        <v>1862.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -1988,7 +1963,7 @@
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D64" s="4">
         <f>C62-G51</f>
-        <v>1665.1699999999998</v>
+        <v>3327.37</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
@@ -1997,7 +1972,7 @@
       </c>
       <c r="D65" s="14">
         <f>C40+C41</f>
-        <v>2065.2200000000003</v>
+        <v>541.44000000000005</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
@@ -2006,7 +1981,7 @@
       </c>
       <c r="D68" s="15">
         <f>D64-D65</f>
-        <v>-400.05000000000041</v>
+        <v>2785.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do projeto express estudos
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemos\Desktop\Projetos\Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9CF1FB-78F5-44FE-B513-ED22470D440B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D77B6A-4D3E-4AD4-9C03-7F95780C91DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>Total</t>
   </si>
@@ -91,9 +91,6 @@
     <t>CAPACETE</t>
   </si>
   <si>
-    <t>PNEU</t>
-  </si>
-  <si>
     <t>IMPRESSORA</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>GASTOS</t>
   </si>
   <si>
-    <t>ROUPA JULIA</t>
-  </si>
-  <si>
     <t>DIA 18</t>
   </si>
   <si>
@@ -184,13 +178,31 @@
     <t>PRODUTOS</t>
   </si>
   <si>
-    <t>TENHO</t>
-  </si>
-  <si>
-    <t>PRECISAR</t>
-  </si>
-  <si>
-    <t>VALOR FATURA</t>
+    <t xml:space="preserve">Tonny </t>
+  </si>
+  <si>
+    <t>Fevereiro</t>
+  </si>
+  <si>
+    <t>Março</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Maio</t>
+  </si>
+  <si>
+    <t>Junho</t>
+  </si>
+  <si>
+    <t>Julho</t>
+  </si>
+  <si>
+    <t>FUTEBOL</t>
+  </si>
+  <si>
+    <t>COMPLEMENTO</t>
   </si>
 </sst>
 </file>
@@ -298,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -337,12 +349,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,26 +632,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="1"/>
+    <col min="15" max="15" width="16.7109375" style="1"/>
     <col min="16" max="16" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="16.42578125" style="1"/>
+    <col min="17" max="16384" width="16.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
@@ -689,14 +694,12 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3">
-        <v>47.01</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="3">
         <v>47.01</v>
       </c>
@@ -732,19 +735,17 @@
       </c>
       <c r="P3" s="4">
         <f>SUM(C3:O3)</f>
-        <v>564.12</v>
+        <v>517.11</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="3">
-        <v>680</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3">
         <v>680</v>
       </c>
@@ -780,19 +781,17 @@
       </c>
       <c r="P4" s="4">
         <f>SUM(C4:O4)</f>
-        <v>8160</v>
+        <v>7480</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3">
-        <v>97.87</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3">
         <v>100</v>
       </c>
@@ -828,20 +827,18 @@
       </c>
       <c r="P5" s="4">
         <f>SUM(C5:O5)</f>
-        <v>1197.8699999999999</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <v>50</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3">
         <v>50</v>
       </c>
@@ -874,19 +871,17 @@
       </c>
       <c r="P6" s="4">
         <f>SUM(C6:O6)</f>
-        <v>550</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="3">
-        <v>100</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3">
         <v>100</v>
       </c>
@@ -922,58 +917,58 @@
       </c>
       <c r="P7" s="4">
         <f>SUM(C7:O7)</f>
-        <v>1200</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="N8" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" ref="P8" si="0">SUM(C8:O8)</f>
-        <v>715</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1015,55 +1010,55 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11" s="5">
         <f t="shared" ref="C11:N11" si="2">SUM(C3:C10)</f>
-        <v>924.88</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="2"/>
-        <v>1042.01</v>
+        <v>987.01</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="2"/>
-        <v>1342.01</v>
+        <v>1337.01</v>
       </c>
       <c r="P11" s="4">
         <f>SUM(C11:O11)</f>
-        <v>15386.990000000002</v>
+        <v>14357.11</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1073,9 +1068,7 @@
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="7">
-        <v>622.55999999999995</v>
-      </c>
+      <c r="C13" s="13"/>
       <c r="D13" s="3">
         <v>622.55999999999995</v>
       </c>
@@ -1096,7 +1089,7 @@
       </c>
       <c r="P13" s="4">
         <f>SUM(C13:O13)</f>
-        <v>4357.92</v>
+        <v>3735.3599999999997</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1104,14 +1097,15 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="7">
-        <v>135</v>
+        <v>55</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="3">
+        <v>29.9</v>
       </c>
       <c r="P15" s="4">
         <f>SUM(C15:O15)</f>
-        <v>135</v>
+        <v>29.9</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1119,17 +1113,24 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7">
-        <v>29.9</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C16" s="13"/>
       <c r="D16" s="3">
-        <v>29.9</v>
+        <v>95.09</v>
+      </c>
+      <c r="E16" s="3">
+        <v>95.09</v>
+      </c>
+      <c r="F16" s="3">
+        <v>95.09</v>
+      </c>
+      <c r="G16" s="3">
+        <v>95.09</v>
       </c>
       <c r="P16" s="4">
         <f>SUM(C16:O16)</f>
-        <v>59.8</v>
+        <v>380.36</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1137,129 +1138,138 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7">
-        <v>34.159999999999997</v>
-      </c>
-      <c r="P17" s="4">
-        <f>SUM(C17:O17)</f>
-        <v>34.159999999999997</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="3">
+        <v>119.7</v>
+      </c>
+      <c r="E17" s="3">
+        <v>119.7</v>
+      </c>
+      <c r="F17" s="3">
+        <v>119.7</v>
+      </c>
+      <c r="G17" s="3">
+        <v>119.7</v>
+      </c>
+      <c r="P17" s="4"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="7">
-        <v>95.09</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="3">
-        <v>95.09</v>
-      </c>
-      <c r="E18" s="3">
-        <v>95.09</v>
-      </c>
-      <c r="F18" s="3">
-        <v>95.09</v>
-      </c>
-      <c r="G18" s="3">
-        <v>95.09</v>
-      </c>
-      <c r="P18" s="4">
-        <f>SUM(C18:O18)</f>
-        <v>475.45000000000005</v>
-      </c>
+        <v>39.270000000000003</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="P18" s="4"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="7">
-        <v>119.7</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="3">
-        <v>119.7</v>
-      </c>
-      <c r="E19" s="3">
-        <v>119.7</v>
-      </c>
-      <c r="F19" s="3">
-        <v>119.7</v>
-      </c>
-      <c r="G19" s="3">
-        <v>119.7</v>
-      </c>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="7">
-        <v>279.95999999999998</v>
-      </c>
-      <c r="D20" s="3">
         <v>1144.92</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="P20" s="4">
-        <f>SUM(C20:O20)</f>
-        <v>1424.88</v>
-      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="P19" s="4">
+        <f>SUM(C19:O19)</f>
+        <v>1144.92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7">
+        <v>871.55</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="P21" s="4"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7">
-        <v>115.33</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="3">
+        <v>135</v>
+      </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="7">
-        <v>135</v>
-      </c>
-      <c r="D23" s="3">
-        <v>135</v>
-      </c>
-      <c r="P23" s="4"/>
-    </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>3</v>
+      <c r="A24" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="7">
-        <v>512</v>
+        <v>22</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="E24" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="F24" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="G24" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="H24" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="I24" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="J24" s="3">
+        <v>331.21</v>
       </c>
       <c r="P24" s="4">
         <f>SUM(C24:O24)</f>
-        <v>512</v>
+        <v>2318.4699999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="3">
+        <v>76.650000000000006</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="P25" s="4">
+        <f>SUM(C25:O25)</f>
+        <v>76.650000000000006</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -1267,33 +1277,23 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C26" s="13"/>
       <c r="D26" s="3">
-        <v>331.21</v>
+        <v>150</v>
       </c>
       <c r="E26" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="F26" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="G26" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="H26" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="I26" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="J26" s="3">
-        <v>331.21</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
       <c r="P26" s="4">
         <f>SUM(C26:O26)</f>
-        <v>2318.4699999999998</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -1301,11 +1301,11 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C27" s="13"/>
       <c r="D27" s="3">
-        <v>30.65</v>
+        <v>86.66</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1313,50 +1313,44 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
-      <c r="P27" s="4">
-        <f>SUM(C27:O27)</f>
-        <v>30.65</v>
-      </c>
+      <c r="P27" s="4"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="13"/>
       <c r="D28" s="3">
-        <v>150</v>
-      </c>
-      <c r="E28" s="3">
-        <v>150</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="P28" s="4">
-        <f>SUM(C28:O28)</f>
-        <v>300</v>
-      </c>
+      <c r="P28" s="4"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="C29" s="13"/>
       <c r="D29" s="3">
-        <v>86.66</v>
+        <v>528.04</v>
       </c>
       <c r="E29" s="3">
-        <v>86.66</v>
-      </c>
-      <c r="F29" s="3"/>
+        <v>528.04</v>
+      </c>
+      <c r="F29" s="3">
+        <v>528.04</v>
+      </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1368,13 +1362,15 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="C30" s="13"/>
       <c r="D30" s="3">
-        <v>420</v>
-      </c>
-      <c r="E30" s="3"/>
+        <v>107.49</v>
+      </c>
+      <c r="E30" s="3">
+        <v>107.49</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1387,284 +1383,282 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C31" s="13"/>
       <c r="D31" s="3">
-        <v>528.04</v>
-      </c>
-      <c r="E31" s="3">
-        <v>528.04</v>
-      </c>
-      <c r="F31" s="3">
-        <v>528.04</v>
-      </c>
+        <v>270.48</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="3">
-        <v>107.49</v>
-      </c>
-      <c r="E32" s="3">
-        <v>107.49</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="3">
-        <v>270.48</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" s="5">
-        <f t="shared" ref="C35:N35" si="3">SUM(C13:C33)</f>
-        <v>2078.6999999999998</v>
-      </c>
-      <c r="D35" s="5">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5">
+        <f t="shared" ref="C33:N33" si="3">SUM(C13:C31)</f>
+        <v>871.55</v>
+      </c>
+      <c r="D33" s="5">
         <f t="shared" si="3"/>
-        <v>4071.7</v>
-      </c>
-      <c r="E35" s="5">
+        <v>4156.9699999999993</v>
+      </c>
+      <c r="E33" s="5">
         <f t="shared" si="3"/>
-        <v>2040.75</v>
-      </c>
-      <c r="F35" s="5">
+        <v>1954.09</v>
+      </c>
+      <c r="F33" s="5">
         <f t="shared" si="3"/>
         <v>1696.6</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G33" s="5">
         <f t="shared" si="3"/>
         <v>1168.56</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H33" s="5">
         <f t="shared" si="3"/>
         <v>953.77</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I33" s="5">
         <f t="shared" si="3"/>
         <v>953.77</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J33" s="5">
         <f t="shared" si="3"/>
         <v>331.21</v>
       </c>
-      <c r="K35" s="5">
+      <c r="K33" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L33" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M33" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N35" s="5">
+      <c r="N33" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P35" s="12">
-        <f>SUM(P13:P33)</f>
-        <v>9648.33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C37" s="12">
-        <f t="shared" ref="C37:N37" si="4">C11+C35</f>
-        <v>3003.58</v>
-      </c>
-      <c r="D37" s="12">
+      <c r="P33" s="12">
+        <f>SUM(P13:P31)</f>
+        <v>7985.66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C35" s="12">
+        <f t="shared" ref="C35:N35" si="4">C11+C33</f>
+        <v>871.55</v>
+      </c>
+      <c r="D35" s="12">
         <f t="shared" si="4"/>
-        <v>5113.71</v>
-      </c>
-      <c r="E37" s="12">
+        <v>5143.9799999999996</v>
+      </c>
+      <c r="E35" s="12">
         <f t="shared" si="4"/>
-        <v>3382.76</v>
-      </c>
-      <c r="F37" s="12">
+        <v>3291.1</v>
+      </c>
+      <c r="F35" s="12">
         <f t="shared" si="4"/>
-        <v>3038.6099999999997</v>
-      </c>
-      <c r="G37" s="12">
+        <v>3033.6099999999997</v>
+      </c>
+      <c r="G35" s="12">
         <f t="shared" si="4"/>
-        <v>2510.5699999999997</v>
-      </c>
-      <c r="H37" s="12">
+        <v>2505.5699999999997</v>
+      </c>
+      <c r="H35" s="12">
         <f t="shared" si="4"/>
-        <v>2295.7799999999997</v>
-      </c>
-      <c r="I37" s="12">
+        <v>2290.7799999999997</v>
+      </c>
+      <c r="I35" s="12">
         <f t="shared" si="4"/>
-        <v>2295.7799999999997</v>
-      </c>
-      <c r="J37" s="12">
+        <v>2290.7799999999997</v>
+      </c>
+      <c r="J35" s="12">
         <f t="shared" si="4"/>
-        <v>1673.22</v>
-      </c>
-      <c r="K37" s="12">
+        <v>1668.22</v>
+      </c>
+      <c r="K35" s="12">
         <f t="shared" si="4"/>
-        <v>1342.01</v>
-      </c>
-      <c r="L37" s="12">
+        <v>1337.01</v>
+      </c>
+      <c r="L35" s="12">
         <f t="shared" si="4"/>
-        <v>1342.01</v>
-      </c>
-      <c r="M37" s="12">
+        <v>1337.01</v>
+      </c>
+      <c r="M35" s="12">
         <f t="shared" si="4"/>
-        <v>1342.01</v>
-      </c>
-      <c r="N37" s="12">
+        <v>1337.01</v>
+      </c>
+      <c r="N35" s="12">
         <f t="shared" si="4"/>
-        <v>1342.01</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1337.01</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="H37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="I37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="J37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="L37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="M37" s="3">
+        <v>2500</v>
+      </c>
+      <c r="N37" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <f>C45</f>
+        <v>5.3500000000000227</v>
+      </c>
+      <c r="E38" s="3">
+        <f t="shared" ref="E38:N38" si="5">D45</f>
+        <v>848.26000000000022</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="5"/>
+        <v>57.160000000000309</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="5"/>
+        <v>2523.5500000000002</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="5"/>
+        <v>2517.9800000000005</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="5"/>
+        <v>2727.2000000000007</v>
+      </c>
+      <c r="J38" s="3">
+        <f t="shared" si="5"/>
+        <v>2936.420000000001</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" si="5"/>
+        <v>3768.2000000000007</v>
+      </c>
+      <c r="L38" s="3">
+        <f t="shared" si="5"/>
+        <v>4931.1900000000005</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" si="5"/>
+        <v>6094.18</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" si="5"/>
+        <v>7257.17</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="D39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="E39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="G39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="H39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="I39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="J39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="K39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="L39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="M39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="N39" s="3">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <v>876.9</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="P39" s="4">
+        <f>P33+P11</f>
+        <v>22342.77</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="3">
-        <v>541.44000000000005</v>
-      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="3">
-        <f t="shared" ref="D40:N40" si="5">C47</f>
-        <v>37.860000000000127</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" si="5"/>
-        <v>856.76999999999953</v>
-      </c>
-      <c r="F40" s="3">
-        <f t="shared" si="5"/>
-        <v>-25.990000000000691</v>
-      </c>
-      <c r="G40" s="3">
-        <f t="shared" si="5"/>
-        <v>2435.3999999999996</v>
-      </c>
-      <c r="H40" s="3">
-        <f t="shared" si="5"/>
-        <v>2424.83</v>
-      </c>
-      <c r="I40" s="3">
-        <f t="shared" si="5"/>
-        <v>2629.05</v>
-      </c>
-      <c r="J40" s="3">
-        <f t="shared" si="5"/>
-        <v>2833.2700000000004</v>
-      </c>
-      <c r="K40" s="3">
-        <f t="shared" si="5"/>
-        <v>3660.05</v>
-      </c>
-      <c r="L40" s="3">
-        <f t="shared" si="5"/>
-        <v>4818.04</v>
-      </c>
-      <c r="M40" s="3">
-        <f t="shared" si="5"/>
-        <v>5976.03</v>
-      </c>
-      <c r="N40" s="3">
-        <f t="shared" si="5"/>
-        <v>7134.0199999999986</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3">
+        <v>3286.89</v>
+      </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3">
+        <v>3000</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -1672,220 +1666,247 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="P41" s="4">
-        <f>P35+P11</f>
-        <v>25035.32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="N41" s="3">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3">
+      <c r="C43" s="7">
+        <f t="shared" ref="C43:N43" si="6">SUM(C37:C41)</f>
+        <v>876.9</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="6"/>
+        <v>5992.24</v>
+      </c>
+      <c r="E43" s="7">
+        <f t="shared" si="6"/>
+        <v>3348.26</v>
+      </c>
+      <c r="F43" s="7">
+        <f t="shared" si="6"/>
+        <v>5557.16</v>
+      </c>
+      <c r="G43" s="7">
+        <f t="shared" si="6"/>
+        <v>5023.55</v>
+      </c>
+      <c r="H43" s="7">
+        <f t="shared" si="6"/>
+        <v>5017.9800000000005</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="6"/>
+        <v>5227.2000000000007</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="6"/>
+        <v>5436.420000000001</v>
+      </c>
+      <c r="K43" s="7">
+        <f t="shared" si="6"/>
+        <v>6268.2000000000007</v>
+      </c>
+      <c r="L43" s="7">
+        <f t="shared" si="6"/>
+        <v>7431.1900000000005</v>
+      </c>
+      <c r="M43" s="7">
+        <f t="shared" si="6"/>
+        <v>8594.18</v>
+      </c>
+      <c r="N43" s="7">
+        <f t="shared" si="6"/>
+        <v>12557.17</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="5">
+        <f t="shared" ref="C45:N45" si="7">C43-C35</f>
+        <v>5.3500000000000227</v>
+      </c>
+      <c r="D45" s="5">
+        <f t="shared" si="7"/>
+        <v>848.26000000000022</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="7"/>
+        <v>57.160000000000309</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" si="7"/>
+        <v>2523.5500000000002</v>
+      </c>
+      <c r="G45" s="5">
+        <f t="shared" si="7"/>
+        <v>2517.9800000000005</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="7"/>
+        <v>2727.2000000000007</v>
+      </c>
+      <c r="I45" s="5">
+        <f t="shared" si="7"/>
+        <v>2936.420000000001</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" si="7"/>
+        <v>3768.2000000000007</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="7"/>
+        <v>4931.1900000000005</v>
+      </c>
+      <c r="L45" s="5">
+        <f t="shared" si="7"/>
+        <v>6094.18</v>
+      </c>
+      <c r="M45" s="5">
+        <f t="shared" si="7"/>
+        <v>7257.17</v>
+      </c>
+      <c r="N45" s="5">
+        <f t="shared" si="7"/>
+        <v>11220.16</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="3">
+        <v>577.20000000000005</v>
+      </c>
+      <c r="D49" s="3">
+        <v>828</v>
+      </c>
+      <c r="E49" s="3">
+        <v>257</v>
+      </c>
+      <c r="F49" s="3">
         <v>200</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3">
-        <v>3232.62</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3">
-        <v>3000</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="7">
-        <f t="shared" ref="C45:N45" si="6">SUM(C39:C43)</f>
-        <v>3041.44</v>
-      </c>
-      <c r="D45" s="7">
-        <f t="shared" si="6"/>
-        <v>5970.48</v>
-      </c>
-      <c r="E45" s="7">
-        <f t="shared" si="6"/>
-        <v>3356.7699999999995</v>
-      </c>
-      <c r="F45" s="7">
-        <f t="shared" si="6"/>
-        <v>5474.0099999999993</v>
-      </c>
-      <c r="G45" s="7">
-        <f t="shared" si="6"/>
-        <v>4935.3999999999996</v>
-      </c>
-      <c r="H45" s="7">
-        <f t="shared" si="6"/>
-        <v>4924.83</v>
-      </c>
-      <c r="I45" s="7">
-        <f t="shared" si="6"/>
-        <v>5129.05</v>
-      </c>
-      <c r="J45" s="7">
-        <f t="shared" si="6"/>
-        <v>5333.27</v>
-      </c>
-      <c r="K45" s="7">
-        <f t="shared" si="6"/>
-        <v>6160.05</v>
-      </c>
-      <c r="L45" s="7">
-        <f t="shared" si="6"/>
-        <v>7318.04</v>
-      </c>
-      <c r="M45" s="7">
-        <f t="shared" si="6"/>
-        <v>8476.0299999999988</v>
-      </c>
-      <c r="N45" s="7">
-        <f t="shared" si="6"/>
-        <v>12434.019999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" s="5">
-        <f t="shared" ref="C47:N47" si="7">C45-C37</f>
-        <v>37.860000000000127</v>
-      </c>
-      <c r="D47" s="5">
-        <f t="shared" si="7"/>
-        <v>856.76999999999953</v>
-      </c>
-      <c r="E47" s="5">
-        <f t="shared" si="7"/>
-        <v>-25.990000000000691</v>
-      </c>
-      <c r="F47" s="5">
-        <f t="shared" si="7"/>
-        <v>2435.3999999999996</v>
-      </c>
-      <c r="G47" s="5">
-        <f t="shared" si="7"/>
-        <v>2424.83</v>
-      </c>
-      <c r="H47" s="5">
-        <f t="shared" si="7"/>
-        <v>2629.05</v>
-      </c>
-      <c r="I47" s="5">
-        <f t="shared" si="7"/>
-        <v>2833.2700000000004</v>
-      </c>
-      <c r="J47" s="5">
-        <f t="shared" si="7"/>
-        <v>3660.05</v>
-      </c>
-      <c r="K47" s="5">
-        <f t="shared" si="7"/>
-        <v>4818.04</v>
-      </c>
-      <c r="L47" s="5">
-        <f t="shared" si="7"/>
-        <v>5976.03</v>
-      </c>
-      <c r="M47" s="5">
-        <f t="shared" si="7"/>
-        <v>7134.0199999999986</v>
-      </c>
-      <c r="N47" s="5">
-        <f t="shared" si="7"/>
-        <v>11092.009999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D49" s="4"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G49" s="3">
+        <f>SUM(C49:F49)</f>
+        <v>1862.2</v>
+      </c>
+      <c r="H49" s="3"/>
+      <c r="J49" s="3">
+        <v>275</v>
+      </c>
+      <c r="L49" s="5">
+        <f>SUM(G49:J49)</f>
+        <v>2137.1999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3">
+        <v>828</v>
+      </c>
+      <c r="E50" s="3">
+        <v>257</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3">
+        <f t="shared" ref="G50:G54" si="8">SUM(C50:F50)</f>
+        <v>1085</v>
+      </c>
+      <c r="J50" s="3">
+        <v>275</v>
+      </c>
+      <c r="L50" s="5">
+        <f t="shared" ref="L50:L54" si="9">SUM(G50:J50)</f>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="E51" s="3">
+        <v>257</v>
+      </c>
       <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="J51" s="5">
-        <f>G51+H51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C52" s="3">
-        <v>577.20000000000005</v>
-      </c>
-      <c r="D52" s="3">
-        <v>828</v>
-      </c>
+      <c r="G51" s="3">
+        <f t="shared" si="8"/>
+        <v>257</v>
+      </c>
+      <c r="J51" s="3">
+        <v>275</v>
+      </c>
+      <c r="L51" s="5">
+        <f t="shared" si="9"/>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
       <c r="E52" s="3">
         <v>257</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3">
-        <f t="shared" ref="G52:G57" si="8">SUM(C52:E52)</f>
-        <v>1662.2</v>
-      </c>
-      <c r="H52" s="3">
-        <v>200</v>
-      </c>
-      <c r="J52" s="5">
-        <f t="shared" ref="J52:J57" si="9">G52+H52</f>
-        <v>1862.2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>257</v>
+      </c>
+      <c r="J52" s="3">
+        <v>275</v>
+      </c>
+      <c r="L52" s="5">
+        <f t="shared" si="9"/>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="3">
-        <v>828</v>
-      </c>
+      <c r="D53" s="3"/>
       <c r="E53" s="3">
         <v>257</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3">
         <f t="shared" si="8"/>
-        <v>1085</v>
-      </c>
-      <c r="J53" s="5">
+        <v>257</v>
+      </c>
+      <c r="L53" s="5">
         <f t="shared" si="9"/>
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3">
@@ -1896,93 +1917,35 @@
         <f t="shared" si="8"/>
         <v>257</v>
       </c>
-      <c r="J54" s="5">
+      <c r="L54" s="5">
         <f t="shared" si="9"/>
         <v>257</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C55" s="3"/>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D55" s="3"/>
-      <c r="E55" s="3">
-        <v>257</v>
-      </c>
+      <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="J55" s="5">
-        <f t="shared" si="9"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3">
-        <v>257</v>
-      </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="J56" s="5">
-        <f t="shared" si="9"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3">
-        <v>257</v>
-      </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="J57" s="5">
-        <f t="shared" si="9"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C58" s="3"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C62" s="1">
-        <v>3327.37</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D64" s="4">
-        <f>C62-G51</f>
-        <v>3327.37</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="14">
-        <f>C40+C41</f>
-        <v>541.44000000000005</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D68" s="15">
-        <f>D64-D65</f>
-        <v>2785.93</v>
-      </c>
+      <c r="G55" s="3"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L58" s="4"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D62" s="4"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Atualização de pastas de estudos criação convertendo excel em pdf
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemos\Desktop\Projetos\Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA450D15-AEB3-4F2A-AE0B-C6B7CD541660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB81E210-293F-43BA-B30E-8E0B5DAEF224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>Total</t>
   </si>
@@ -88,9 +88,6 @@
     <t>NOVEMBRO</t>
   </si>
   <si>
-    <t>CAPACETE</t>
-  </si>
-  <si>
     <t>IMPRESSORA</t>
   </si>
   <si>
@@ -209,6 +206,12 @@
   </si>
   <si>
     <t>LIXEIRA</t>
+  </si>
+  <si>
+    <t>BOLSA JULIA</t>
+  </si>
+  <si>
+    <t>ABASTECIMENTO</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -646,7 +649,7 @@
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" style="1"/>
@@ -656,7 +659,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
@@ -700,10 +703,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3">
@@ -746,10 +749,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3">
@@ -792,14 +795,14 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
-        <v>100</v>
+        <v>105.71</v>
       </c>
       <c r="E5" s="3">
         <v>100</v>
@@ -833,15 +836,15 @@
       </c>
       <c r="P5" s="4">
         <f>SUM(C5:O5)</f>
-        <v>1100</v>
+        <v>1105.71</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -882,10 +885,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
@@ -928,10 +931,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
@@ -974,7 +977,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1020,7 +1023,7 @@
       </c>
       <c r="D11" s="5">
         <f t="shared" si="2"/>
-        <v>987.01</v>
+        <v>992.72</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="2"/>
@@ -1064,7 +1067,7 @@
       </c>
       <c r="P11" s="4">
         <f>SUM(C11:O11)</f>
-        <v>14357.11</v>
+        <v>14362.820000000002</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1103,7 +1106,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="3">
@@ -1119,7 +1122,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="3">
@@ -1144,7 +1147,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="3">
@@ -1166,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="3">
@@ -1182,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="3">
@@ -1198,7 +1201,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="3">
@@ -1207,113 +1210,98 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="P20" s="4">
-        <f>SUM(C20:O20)</f>
-        <v>1144.92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="3"/>
-      <c r="P22" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="3">
+        <v>54.195</v>
+      </c>
+      <c r="E21" s="3">
+        <v>54.195</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="P21" s="4">
+        <f>SUM(C21:O21)</f>
+        <v>108.39</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="3">
-        <v>135</v>
+        <v>109.51</v>
       </c>
       <c r="P23" s="4"/>
     </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="3">
+        <v>58.06</v>
+      </c>
+      <c r="P24" s="4"/>
+    </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>4</v>
+      <c r="A25" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="E25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="F25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="G25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="H25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="I25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="J25" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="P25" s="4">
-        <f>SUM(C25:O25)</f>
-        <v>2318.4699999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="3">
-        <v>76.650000000000006</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="P26" s="4">
-        <f>SUM(C26:O26)</f>
-        <v>76.650000000000006</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="P25" s="4"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="3">
-        <v>150</v>
+        <v>331.21</v>
       </c>
       <c r="E27" s="3">
-        <v>150</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+        <v>331.21</v>
+      </c>
+      <c r="F27" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="G27" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="H27" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="I27" s="3">
+        <v>331.21</v>
+      </c>
+      <c r="J27" s="3">
+        <v>331.21</v>
+      </c>
       <c r="P27" s="4">
         <f>SUM(C27:O27)</f>
-        <v>300</v>
+        <v>2318.4699999999998</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -1321,11 +1309,11 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="3">
-        <v>86.66</v>
+        <v>76.650000000000006</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1333,44 +1321,48 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="P28" s="4"/>
+      <c r="P28" s="4">
+        <f>SUM(C28:O28)</f>
+        <v>76.650000000000006</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="3">
-        <v>420</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="E29" s="3">
+        <v>150</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="P29" s="4"/>
+      <c r="P29" s="4">
+        <f>SUM(C29:O29)</f>
+        <v>300</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="3">
-        <v>528.04</v>
-      </c>
-      <c r="E30" s="3">
-        <v>528.04</v>
-      </c>
-      <c r="F30" s="3">
-        <v>528.04</v>
-      </c>
+        <v>86.66</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1382,15 +1374,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="3">
-        <v>107.49</v>
-      </c>
-      <c r="E31" s="3">
-        <v>107.49</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1403,14 +1393,18 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="3">
-        <v>270.48</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+        <v>528.04</v>
+      </c>
+      <c r="E32" s="3">
+        <v>528.04</v>
+      </c>
+      <c r="F32" s="3">
+        <v>528.04</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -1422,13 +1416,15 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="3">
-        <v>55.6</v>
-      </c>
-      <c r="E33" s="3"/>
+        <v>107.49</v>
+      </c>
+      <c r="E33" s="3">
+        <v>107.49</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -1436,265 +1432,259 @@
       <c r="J33" s="3"/>
       <c r="P33" s="4"/>
     </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="3">
+        <v>270.48</v>
+      </c>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="P34" s="4"/>
+    </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
-      <c r="C35" s="5">
-        <f t="shared" ref="C35:N35" si="3">SUM(C13:C33)</f>
+      <c r="A35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="3">
+        <v>55.6</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="P35" s="4"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="5">
+        <f t="shared" ref="C37:N37" si="3">SUM(C13:C35)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D37" s="5">
         <f t="shared" si="3"/>
-        <v>4253.9400000000005</v>
-      </c>
-      <c r="E35" s="5">
+        <v>4475.7049999999999</v>
+      </c>
+      <c r="E37" s="5">
         <f t="shared" si="3"/>
-        <v>1954.09</v>
-      </c>
-      <c r="F35" s="5">
+        <v>2008.2850000000001</v>
+      </c>
+      <c r="F37" s="5">
         <f t="shared" si="3"/>
         <v>1696.6</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G37" s="5">
         <f t="shared" si="3"/>
         <v>1168.56</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H37" s="5">
         <f t="shared" si="3"/>
         <v>953.77</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I37" s="5">
         <f t="shared" si="3"/>
         <v>953.77</v>
       </c>
-      <c r="J35" s="5">
+      <c r="J37" s="5">
         <f t="shared" si="3"/>
         <v>331.21</v>
       </c>
-      <c r="K35" s="5">
+      <c r="K37" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L37" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M35" s="5">
+      <c r="M37" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N35" s="5">
+      <c r="N37" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P35" s="12">
-        <f>SUM(P13:P33)</f>
-        <v>7985.66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C37" s="12">
-        <f t="shared" ref="C37:N37" si="4">C11+C35</f>
+      <c r="P37" s="12">
+        <f>SUM(P13:P35)</f>
+        <v>6949.1299999999992</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C39" s="12">
+        <f t="shared" ref="C39:N39" si="4">C11+C37</f>
         <v>0</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D39" s="12">
         <f t="shared" si="4"/>
-        <v>5240.9500000000007</v>
-      </c>
-      <c r="E37" s="12">
+        <v>5468.4250000000002</v>
+      </c>
+      <c r="E39" s="12">
         <f t="shared" si="4"/>
-        <v>3291.1</v>
-      </c>
-      <c r="F37" s="12">
+        <v>3345.2950000000001</v>
+      </c>
+      <c r="F39" s="12">
         <f t="shared" si="4"/>
         <v>3033.6099999999997</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G39" s="12">
         <f t="shared" si="4"/>
         <v>2505.5699999999997</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H39" s="12">
         <f t="shared" si="4"/>
         <v>2290.7799999999997</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I39" s="12">
         <f t="shared" si="4"/>
         <v>2290.7799999999997</v>
       </c>
-      <c r="J37" s="12">
+      <c r="J39" s="12">
         <f t="shared" si="4"/>
         <v>1668.22</v>
       </c>
-      <c r="K37" s="12">
+      <c r="K39" s="12">
         <f t="shared" si="4"/>
         <v>1337.01</v>
       </c>
-      <c r="L37" s="12">
+      <c r="L39" s="12">
         <f t="shared" si="4"/>
         <v>1337.01</v>
       </c>
-      <c r="M37" s="12">
+      <c r="M39" s="12">
         <f t="shared" si="4"/>
         <v>1337.01</v>
       </c>
-      <c r="N37" s="12">
+      <c r="N39" s="12">
         <f t="shared" si="4"/>
         <v>1337.01</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="E39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="F39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="G39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="H39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="I39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="J39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="K39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="L39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="M39" s="3">
-        <v>2500</v>
-      </c>
-      <c r="N39" s="3">
-        <v>2500</v>
-      </c>
-    </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3">
-        <v>6.28</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" ref="E40:N40" si="5">D47</f>
-        <v>752.21999999999935</v>
-      </c>
-      <c r="F40" s="3">
-        <f t="shared" si="5"/>
-        <v>-38.880000000000564</v>
-      </c>
-      <c r="G40" s="3">
-        <f t="shared" si="5"/>
-        <v>2427.5099999999993</v>
-      </c>
-      <c r="H40" s="3">
-        <f t="shared" si="5"/>
-        <v>2421.9399999999996</v>
-      </c>
-      <c r="I40" s="3">
-        <f t="shared" si="5"/>
-        <v>2631.16</v>
-      </c>
-      <c r="J40" s="3">
-        <f t="shared" si="5"/>
-        <v>2840.38</v>
-      </c>
-      <c r="K40" s="3">
-        <f t="shared" si="5"/>
-        <v>3672.16</v>
-      </c>
-      <c r="L40" s="3">
-        <f t="shared" si="5"/>
-        <v>4835.1499999999996</v>
-      </c>
-      <c r="M40" s="3">
-        <f t="shared" si="5"/>
-        <v>5998.1399999999994</v>
-      </c>
-      <c r="N40" s="3">
-        <f t="shared" si="5"/>
-        <v>7161.1299999999992</v>
-      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="P41" s="4">
-        <f>P35+P11</f>
-        <v>22342.77</v>
+      <c r="D41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="E41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="F41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="G41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="H41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="J41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="K41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="L41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="M41" s="3">
+        <v>2300</v>
+      </c>
+      <c r="N41" s="3">
+        <v>2300</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3">
-        <v>200</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
+        <v>6.28</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" ref="E42:N42" si="5">D49</f>
+        <v>324.74499999999989</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="5"/>
+        <v>-720.55000000000018</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="5"/>
+        <v>1545.8400000000001</v>
+      </c>
+      <c r="H42" s="3">
+        <f t="shared" si="5"/>
+        <v>1340.2700000000004</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="5"/>
+        <v>1349.4900000000007</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="5"/>
+        <v>1358.7100000000009</v>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" si="5"/>
+        <v>1990.4900000000009</v>
+      </c>
+      <c r="L42" s="3">
+        <f t="shared" si="5"/>
+        <v>2953.4800000000005</v>
+      </c>
+      <c r="M42" s="3">
+        <f t="shared" si="5"/>
+        <v>3916.4700000000003</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" si="5"/>
+        <v>4879.46</v>
+      </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="3">
-        <v>3286.89</v>
-      </c>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3">
-        <v>3000</v>
-      </c>
+      <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -1702,286 +1692,330 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="3">
+      <c r="N43" s="3"/>
+      <c r="P43" s="4">
+        <f>P37+P11</f>
+        <v>21311.95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3">
+        <v>200</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3">
+        <v>3286.89</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3">
+        <v>3000</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3">
         <v>2800</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" ref="C47:N47" si="6">SUM(C41:C45)</f>
+        <v>0</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="6"/>
+        <v>5793.17</v>
+      </c>
+      <c r="E47" s="7">
+        <f t="shared" si="6"/>
+        <v>2624.7449999999999</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="6"/>
+        <v>4579.45</v>
+      </c>
+      <c r="G47" s="7">
+        <f t="shared" si="6"/>
+        <v>3845.84</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="6"/>
+        <v>3640.2700000000004</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="6"/>
+        <v>3649.4900000000007</v>
+      </c>
+      <c r="J47" s="7">
+        <f t="shared" si="6"/>
+        <v>3658.7100000000009</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="6"/>
+        <v>4290.4900000000007</v>
+      </c>
+      <c r="L47" s="7">
+        <f t="shared" si="6"/>
+        <v>5253.4800000000005</v>
+      </c>
+      <c r="M47" s="7">
+        <f t="shared" si="6"/>
+        <v>6216.47</v>
+      </c>
+      <c r="N47" s="7">
+        <f t="shared" si="6"/>
+        <v>9979.4599999999991</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="7">
-        <f t="shared" ref="C45:N45" si="6">SUM(C39:C43)</f>
+      <c r="C49" s="5">
+        <f t="shared" ref="C49:N49" si="7">C47-C39</f>
         <v>0</v>
       </c>
-      <c r="D45" s="7">
-        <f t="shared" si="6"/>
-        <v>5993.17</v>
-      </c>
-      <c r="E45" s="7">
-        <f t="shared" si="6"/>
-        <v>3252.2199999999993</v>
-      </c>
-      <c r="F45" s="7">
-        <f t="shared" si="6"/>
-        <v>5461.119999999999</v>
-      </c>
-      <c r="G45" s="7">
-        <f t="shared" si="6"/>
-        <v>4927.5099999999993</v>
-      </c>
-      <c r="H45" s="7">
-        <f t="shared" si="6"/>
-        <v>4921.9399999999996</v>
-      </c>
-      <c r="I45" s="7">
-        <f t="shared" si="6"/>
-        <v>5131.16</v>
-      </c>
-      <c r="J45" s="7">
-        <f t="shared" si="6"/>
-        <v>5340.38</v>
-      </c>
-      <c r="K45" s="7">
-        <f t="shared" si="6"/>
-        <v>6172.16</v>
-      </c>
-      <c r="L45" s="7">
-        <f t="shared" si="6"/>
-        <v>7335.15</v>
-      </c>
-      <c r="M45" s="7">
-        <f t="shared" si="6"/>
-        <v>8498.14</v>
-      </c>
-      <c r="N45" s="7">
-        <f t="shared" si="6"/>
-        <v>12461.13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="5">
-        <f t="shared" ref="C47:N47" si="7">C45-C37</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="5">
+      <c r="D49" s="5">
         <f t="shared" si="7"/>
-        <v>752.21999999999935</v>
-      </c>
-      <c r="E47" s="5">
+        <v>324.74499999999989</v>
+      </c>
+      <c r="E49" s="5">
         <f t="shared" si="7"/>
-        <v>-38.880000000000564</v>
-      </c>
-      <c r="F47" s="5">
+        <v>-720.55000000000018</v>
+      </c>
+      <c r="F49" s="5">
         <f t="shared" si="7"/>
-        <v>2427.5099999999993</v>
-      </c>
-      <c r="G47" s="5">
+        <v>1545.8400000000001</v>
+      </c>
+      <c r="G49" s="5">
         <f t="shared" si="7"/>
-        <v>2421.9399999999996</v>
-      </c>
-      <c r="H47" s="5">
+        <v>1340.2700000000004</v>
+      </c>
+      <c r="H49" s="5">
         <f t="shared" si="7"/>
-        <v>2631.16</v>
-      </c>
-      <c r="I47" s="5">
+        <v>1349.4900000000007</v>
+      </c>
+      <c r="I49" s="5">
         <f t="shared" si="7"/>
-        <v>2840.38</v>
-      </c>
-      <c r="J47" s="5">
+        <v>1358.7100000000009</v>
+      </c>
+      <c r="J49" s="5">
         <f t="shared" si="7"/>
-        <v>3672.16</v>
-      </c>
-      <c r="K47" s="5">
+        <v>1990.4900000000009</v>
+      </c>
+      <c r="K49" s="5">
         <f t="shared" si="7"/>
-        <v>4835.1499999999996</v>
-      </c>
-      <c r="L47" s="5">
+        <v>2953.4800000000005</v>
+      </c>
+      <c r="L49" s="5">
         <f t="shared" si="7"/>
-        <v>5998.1399999999994</v>
-      </c>
-      <c r="M47" s="5">
+        <v>3916.4700000000003</v>
+      </c>
+      <c r="M49" s="5">
         <f t="shared" si="7"/>
-        <v>7161.1299999999992</v>
-      </c>
-      <c r="N47" s="5">
+        <v>4879.46</v>
+      </c>
+      <c r="N49" s="5">
         <f t="shared" si="7"/>
-        <v>11124.119999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J50" s="1" t="s">
+        <v>8642.4499999999989</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+      <c r="E53" s="3">
+        <v>577.20000000000005</v>
+      </c>
+      <c r="F53" s="3">
+        <v>828</v>
+      </c>
+      <c r="G53" s="3">
+        <v>257</v>
+      </c>
+      <c r="H53" s="3">
+        <v>200</v>
+      </c>
+      <c r="I53" s="3">
+        <f>SUM(E53:H53)</f>
+        <v>1862.2</v>
+      </c>
+      <c r="J53" s="3"/>
+      <c r="L53" s="3">
+        <v>275</v>
+      </c>
+      <c r="N53" s="5">
+        <f>SUM(I53:L53)</f>
+        <v>2137.1999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="3">
-        <v>577.20000000000005</v>
-      </c>
-      <c r="D51" s="3">
+      <c r="E54" s="3"/>
+      <c r="F54" s="3">
         <v>828</v>
       </c>
-      <c r="E51" s="3">
+      <c r="G54" s="3">
         <v>257</v>
       </c>
-      <c r="F51" s="3">
-        <v>200</v>
-      </c>
-      <c r="G51" s="3">
-        <f>SUM(C51:F51)</f>
-        <v>1862.2</v>
-      </c>
-      <c r="H51" s="3"/>
-      <c r="J51" s="3">
+      <c r="H54" s="3"/>
+      <c r="I54" s="3">
+        <f t="shared" ref="I54:I58" si="8">SUM(E54:H54)</f>
+        <v>1085</v>
+      </c>
+      <c r="L54" s="3">
         <v>275</v>
       </c>
-      <c r="L51" s="5">
-        <f>SUM(G51:J51)</f>
-        <v>2137.1999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
+      <c r="N54" s="5">
+        <f t="shared" ref="N54:N58" si="9">SUM(I54:L54)</f>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3">
-        <v>828</v>
-      </c>
-      <c r="E52" s="3">
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3">
         <v>257</v>
       </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3">
-        <f t="shared" ref="G52:G56" si="8">SUM(C52:F52)</f>
-        <v>1085</v>
-      </c>
-      <c r="J52" s="3">
-        <v>275</v>
-      </c>
-      <c r="L52" s="5">
-        <f t="shared" ref="L52:L56" si="9">SUM(G52:J52)</f>
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3">
-        <v>257</v>
-      </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3">
+      <c r="H55" s="3"/>
+      <c r="I55" s="3">
         <f t="shared" si="8"/>
         <v>257</v>
       </c>
-      <c r="J53" s="3">
+      <c r="L55" s="3">
         <v>275</v>
       </c>
-      <c r="L53" s="5">
+      <c r="N55" s="5">
         <f t="shared" si="9"/>
         <v>532</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3">
         <v>257</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3">
+      <c r="H56" s="3"/>
+      <c r="I56" s="3">
         <f t="shared" si="8"/>
         <v>257</v>
       </c>
-      <c r="J54" s="3">
+      <c r="L56" s="3">
         <v>275</v>
       </c>
-      <c r="L54" s="5">
+      <c r="N56" s="5">
         <f t="shared" si="9"/>
         <v>532</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3">
         <v>257</v>
       </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3">
+      <c r="H57" s="3"/>
+      <c r="I57" s="3">
         <f t="shared" si="8"/>
         <v>257</v>
       </c>
-      <c r="L55" s="5">
+      <c r="N57" s="5">
         <f t="shared" si="9"/>
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3">
         <v>257</v>
       </c>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3">
+      <c r="H58" s="3"/>
+      <c r="I58" s="3">
         <f t="shared" si="8"/>
         <v>257</v>
       </c>
-      <c r="L56" s="5">
+      <c r="N58" s="5">
         <f t="shared" si="9"/>
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="L57" s="4"/>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L58" s="4"/>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L60" s="4"/>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D64" s="4"/>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="4"/>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L62" s="4"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="4"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Atualização dos estudos --> finalizei uma api-node-mysql
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lemos\Desktop\Projetos\Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB81E210-293F-43BA-B30E-8E0B5DAEF224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46465AA8-76B6-4713-AB88-0AA930FCF2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Total</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>DEZEMBRO</t>
-  </si>
-  <si>
-    <t>JANEIRO</t>
   </si>
   <si>
     <t>FEVEREIRO</t>
@@ -319,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,9 +352,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -641,25 +635,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="1"/>
-    <col min="16" max="16" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="16.7109375" style="1"/>
+    <col min="3" max="12" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="1"/>
+    <col min="15" max="15" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="16.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
@@ -692,23 +685,22 @@
         <v>16</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="C3" s="3">
+        <v>47.01</v>
+      </c>
       <c r="D3" s="3">
         <v>47.01</v>
       </c>
@@ -739,22 +731,21 @@
       <c r="M3" s="3">
         <v>47.01</v>
       </c>
-      <c r="N3" s="3">
-        <v>47.01</v>
-      </c>
-      <c r="P3" s="4">
-        <f>SUM(C3:O3)</f>
+      <c r="O3" s="4">
+        <f>SUM(C3:N3)</f>
         <v>517.11</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C4" s="3">
+        <v>680</v>
+      </c>
       <c r="D4" s="3">
         <v>680</v>
       </c>
@@ -785,69 +776,67 @@
       <c r="M4" s="3">
         <v>680</v>
       </c>
-      <c r="N4" s="3">
-        <v>680</v>
-      </c>
-      <c r="P4" s="4">
-        <f>SUM(C4:O4)</f>
+      <c r="O4" s="4">
+        <f>SUM(C4:N4)</f>
         <v>7480</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3">
+        <v>105.71</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3">
+        <v>100</v>
+      </c>
+      <c r="G5" s="3">
+        <v>100</v>
+      </c>
+      <c r="H5" s="3">
+        <v>100</v>
+      </c>
+      <c r="I5" s="3">
+        <v>100</v>
+      </c>
+      <c r="J5" s="3">
+        <v>100</v>
+      </c>
+      <c r="K5" s="3">
+        <v>100</v>
+      </c>
+      <c r="L5" s="3">
+        <v>100</v>
+      </c>
+      <c r="M5" s="3">
+        <v>100</v>
+      </c>
+      <c r="O5" s="4">
+        <f>SUM(C5:N5)</f>
+        <v>1105.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>105.71</v>
-      </c>
-      <c r="E5" s="3">
-        <v>100</v>
-      </c>
-      <c r="F5" s="3">
-        <v>100</v>
-      </c>
-      <c r="G5" s="3">
-        <v>100</v>
-      </c>
-      <c r="H5" s="3">
-        <v>100</v>
-      </c>
-      <c r="I5" s="3">
-        <v>100</v>
-      </c>
-      <c r="J5" s="3">
-        <v>100</v>
-      </c>
-      <c r="K5" s="3">
-        <v>100</v>
-      </c>
-      <c r="L5" s="3">
-        <v>100</v>
-      </c>
-      <c r="M5" s="3">
-        <v>100</v>
-      </c>
-      <c r="N5" s="3">
-        <v>100</v>
-      </c>
-      <c r="P5" s="4">
-        <f>SUM(C5:O5)</f>
-        <v>1105.71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>50</v>
+      </c>
       <c r="E6" s="3">
         <v>50</v>
       </c>
@@ -875,22 +864,21 @@
       <c r="M6" s="3">
         <v>50</v>
       </c>
-      <c r="N6" s="3">
-        <v>50</v>
-      </c>
-      <c r="P6" s="4">
-        <f>SUM(C6:O6)</f>
+      <c r="O6" s="4">
+        <f>SUM(C6:N6)</f>
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="C7" s="3">
+        <v>100</v>
+      </c>
       <c r="D7" s="3">
         <v>100</v>
       </c>
@@ -921,22 +909,21 @@
       <c r="M7" s="3">
         <v>100</v>
       </c>
-      <c r="N7" s="3">
-        <v>100</v>
-      </c>
-      <c r="P7" s="4">
-        <f>SUM(C7:O7)</f>
+      <c r="O7" s="4">
+        <f>SUM(C7:N7)</f>
         <v>1100</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3">
+        <v>60</v>
+      </c>
       <c r="D8" s="3">
         <v>60</v>
       </c>
@@ -967,20 +954,19 @@
       <c r="M8" s="3">
         <v>60</v>
       </c>
-      <c r="N8" s="3">
-        <v>60</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" ref="P8" si="0">SUM(C8:O8)</f>
+      <c r="O8" s="4">
+        <f>SUM(C8:N8)</f>
         <v>660</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3">
+        <v>300</v>
+      </c>
       <c r="E9" s="3">
         <v>300</v>
       </c>
@@ -1008,76 +994,71 @@
       <c r="M9" s="3">
         <v>300</v>
       </c>
-      <c r="N9" s="3">
-        <v>300</v>
-      </c>
-      <c r="P9" s="4">
-        <f t="shared" ref="P9" si="1">SUM(C9:O9)</f>
+      <c r="O9" s="4">
+        <f>SUM(C9:N9)</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="5">
-        <f t="shared" ref="C11:N11" si="2">SUM(C3:C10)</f>
-        <v>0</v>
+        <f t="shared" ref="C11:M11" si="0">SUM(C3:C10)</f>
+        <v>992.72</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="2"/>
-        <v>992.72</v>
+        <f t="shared" si="0"/>
+        <v>1337.01</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="G11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1337.01</v>
       </c>
-      <c r="N11" s="5">
-        <f t="shared" si="2"/>
-        <v>1337.01</v>
-      </c>
-      <c r="P11" s="4">
-        <f>SUM(C11:O11)</f>
+      <c r="O11" s="4">
+        <f>SUM(C11:N11)</f>
         <v>14362.820000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="3">
+        <v>622.55999999999995</v>
+      </c>
       <c r="D13" s="3">
         <v>622.55999999999995</v>
       </c>
@@ -1093,38 +1074,36 @@
       <c r="H13" s="3">
         <v>622.55999999999995</v>
       </c>
-      <c r="I13" s="3">
-        <v>622.55999999999995</v>
-      </c>
-      <c r="P13" s="4">
-        <f>SUM(C13:O13)</f>
+      <c r="O13" s="4">
+        <f>SUM(C13:N13)</f>
         <v>3735.3599999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="3">
+        <v>53</v>
+      </c>
+      <c r="C15" s="3">
         <v>29.9</v>
       </c>
-      <c r="P15" s="4">
-        <f>SUM(C15:O15)</f>
+      <c r="O15" s="4">
+        <f>SUM(C15:N15)</f>
         <v>29.9</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="C16" s="3">
+        <v>95.09</v>
+      </c>
       <c r="D16" s="3">
         <v>95.09</v>
       </c>
@@ -1134,22 +1113,21 @@
       <c r="F16" s="3">
         <v>95.09</v>
       </c>
-      <c r="G16" s="3">
-        <v>95.09</v>
-      </c>
-      <c r="P16" s="4">
-        <f>SUM(C16:O16)</f>
+      <c r="O16" s="4">
+        <f>SUM(C16:N16)</f>
         <v>380.36</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="13"/>
+        <v>18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>119.7</v>
+      </c>
       <c r="D17" s="3">
         <v>119.7</v>
       </c>
@@ -1159,125 +1137,119 @@
       <c r="F17" s="3">
         <v>119.7</v>
       </c>
-      <c r="G17" s="3">
-        <v>119.7</v>
-      </c>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="3">
+        <v>54</v>
+      </c>
+      <c r="C18" s="3">
         <v>39.270000000000003</v>
       </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="3">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3">
         <v>41.37</v>
       </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="3">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3">
         <v>1144.92</v>
       </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="13"/>
+        <v>57</v>
+      </c>
+      <c r="C21" s="3">
+        <v>54.195</v>
+      </c>
       <c r="D21" s="3">
         <v>54.195</v>
       </c>
-      <c r="E21" s="3">
-        <v>54.195</v>
-      </c>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="P21" s="4">
-        <f>SUM(C21:O21)</f>
+      <c r="O21" s="4">
+        <f>SUM(C21:N21)</f>
         <v>108.39</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="3">
-        <v>109.51</v>
-      </c>
-      <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="3">
+        <v>124.51</v>
+      </c>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="3">
+        <v>58</v>
+      </c>
+      <c r="C24" s="3">
         <v>58.06</v>
       </c>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="3">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3">
         <v>135</v>
       </c>
-      <c r="P25" s="4"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O25" s="4"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="3">
+        <v>331.21</v>
+      </c>
       <c r="D27" s="3">
         <v>331.21</v>
       </c>
@@ -1296,286 +1268,267 @@
       <c r="I27" s="3">
         <v>331.21</v>
       </c>
-      <c r="J27" s="3">
-        <v>331.21</v>
-      </c>
-      <c r="P27" s="4">
-        <f>SUM(C27:O27)</f>
+      <c r="O27" s="4">
+        <f>SUM(C27:N27)</f>
         <v>2318.4699999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="3">
+        <v>21</v>
+      </c>
+      <c r="C28" s="3">
         <v>76.650000000000006</v>
       </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="P28" s="4">
-        <f>SUM(C28:O28)</f>
+      <c r="O28" s="4">
+        <f>SUM(C28:N28)</f>
         <v>76.650000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="C29" s="3">
+        <v>150</v>
+      </c>
       <c r="D29" s="3">
         <v>150</v>
       </c>
-      <c r="E29" s="3">
-        <v>150</v>
-      </c>
+      <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="P29" s="4">
-        <f>SUM(C29:O29)</f>
+      <c r="O29" s="4">
+        <f>SUM(C29:N29)</f>
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="3">
+        <v>38</v>
+      </c>
+      <c r="C30" s="3">
         <v>86.66</v>
       </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="3">
+        <v>19</v>
+      </c>
+      <c r="C31" s="3">
         <v>420</v>
       </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="13"/>
+        <v>44</v>
+      </c>
+      <c r="C32" s="3">
+        <v>528.04</v>
+      </c>
       <c r="D32" s="3">
         <v>528.04</v>
       </c>
       <c r="E32" s="3">
         <v>528.04</v>
       </c>
-      <c r="F32" s="3">
-        <v>528.04</v>
-      </c>
+      <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O32" s="4"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="C33" s="3">
+        <v>107.49</v>
+      </c>
       <c r="D33" s="3">
         <v>107.49</v>
       </c>
-      <c r="E33" s="3">
-        <v>107.49</v>
-      </c>
+      <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O33" s="4"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="3">
+        <v>30</v>
+      </c>
+      <c r="C34" s="3">
         <v>270.48</v>
       </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O34" s="4"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="3">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3">
         <v>55.6</v>
       </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O35" s="4"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
       <c r="C37" s="5">
-        <f t="shared" ref="C37:N37" si="3">SUM(C13:C35)</f>
+        <f t="shared" ref="C37:M37" si="1">SUM(C13:C35)</f>
+        <v>4490.7049999999999</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="1"/>
+        <v>2008.2850000000001</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="1"/>
+        <v>1696.6</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="1"/>
+        <v>1168.56</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="1"/>
+        <v>953.77</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="1"/>
+        <v>953.77</v>
+      </c>
+      <c r="I37" s="5">
+        <f t="shared" si="1"/>
+        <v>331.21</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D37" s="5">
-        <f t="shared" si="3"/>
-        <v>4475.7049999999999</v>
-      </c>
-      <c r="E37" s="5">
-        <f t="shared" si="3"/>
-        <v>2008.2850000000001</v>
-      </c>
-      <c r="F37" s="5">
-        <f t="shared" si="3"/>
-        <v>1696.6</v>
-      </c>
-      <c r="G37" s="5">
-        <f t="shared" si="3"/>
-        <v>1168.56</v>
-      </c>
-      <c r="H37" s="5">
-        <f t="shared" si="3"/>
-        <v>953.77</v>
-      </c>
-      <c r="I37" s="5">
-        <f t="shared" si="3"/>
-        <v>953.77</v>
-      </c>
-      <c r="J37" s="5">
-        <f t="shared" si="3"/>
-        <v>331.21</v>
-      </c>
       <c r="K37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N37" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="12">
-        <f>SUM(P13:P35)</f>
+      <c r="O37" s="12">
+        <f>SUM(O13:O35)</f>
         <v>6949.1299999999992</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C39" s="12">
-        <f t="shared" ref="C39:N39" si="4">C11+C37</f>
-        <v>0</v>
+        <f t="shared" ref="C39:M39" si="2">C11+C37</f>
+        <v>5483.4250000000002</v>
       </c>
       <c r="D39" s="12">
-        <f t="shared" si="4"/>
-        <v>5468.4250000000002</v>
+        <f t="shared" si="2"/>
+        <v>3345.2950000000001</v>
       </c>
       <c r="E39" s="12">
-        <f t="shared" si="4"/>
-        <v>3345.2950000000001</v>
+        <f t="shared" si="2"/>
+        <v>3033.6099999999997</v>
       </c>
       <c r="F39" s="12">
-        <f t="shared" si="4"/>
-        <v>3033.6099999999997</v>
+        <f t="shared" si="2"/>
+        <v>2505.5699999999997</v>
       </c>
       <c r="G39" s="12">
-        <f t="shared" si="4"/>
-        <v>2505.5699999999997</v>
+        <f t="shared" si="2"/>
+        <v>2290.7799999999997</v>
       </c>
       <c r="H39" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>2290.7799999999997</v>
       </c>
       <c r="I39" s="12">
-        <f t="shared" si="4"/>
-        <v>2290.7799999999997</v>
+        <f t="shared" si="2"/>
+        <v>1668.22</v>
       </c>
       <c r="J39" s="12">
-        <f t="shared" si="4"/>
-        <v>1668.22</v>
+        <f t="shared" si="2"/>
+        <v>1337.01</v>
       </c>
       <c r="K39" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1337.01</v>
       </c>
       <c r="L39" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1337.01</v>
       </c>
       <c r="M39" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1337.01</v>
       </c>
-      <c r="N39" s="12">
-        <f t="shared" si="4"/>
-        <v>1337.01</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -1587,13 +1540,14 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2300</v>
+      </c>
       <c r="D41" s="3">
         <v>2300</v>
       </c>
@@ -1624,66 +1578,66 @@
       <c r="M41" s="3">
         <v>2300</v>
       </c>
-      <c r="N41" s="3">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="3">
+        <v>6.28</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" ref="D42:M42" si="3">C49</f>
+        <v>309.74499999999989</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="3"/>
+        <v>964.44999999999982</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="3"/>
+        <v>1930.8400000000001</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="3"/>
+        <v>1725.2700000000004</v>
+      </c>
+      <c r="H42" s="3">
+        <f t="shared" si="3"/>
+        <v>1734.4900000000007</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="3"/>
+        <v>1743.7100000000009</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="3"/>
+        <v>2375.4900000000007</v>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" si="3"/>
+        <v>3338.4800000000005</v>
+      </c>
+      <c r="L42" s="3">
+        <f t="shared" si="3"/>
+        <v>4301.47</v>
+      </c>
+      <c r="M42" s="3">
+        <f t="shared" si="3"/>
+        <v>5264.46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3">
-        <v>6.28</v>
-      </c>
-      <c r="E42" s="3">
-        <f t="shared" ref="E42:N42" si="5">D49</f>
-        <v>324.74499999999989</v>
-      </c>
-      <c r="F42" s="3">
-        <f t="shared" si="5"/>
-        <v>-720.55000000000018</v>
-      </c>
-      <c r="G42" s="3">
-        <f t="shared" si="5"/>
-        <v>1545.8400000000001</v>
-      </c>
-      <c r="H42" s="3">
-        <f t="shared" si="5"/>
-        <v>1340.2700000000004</v>
-      </c>
-      <c r="I42" s="3">
-        <f t="shared" si="5"/>
-        <v>1349.4900000000007</v>
-      </c>
-      <c r="J42" s="3">
-        <f t="shared" si="5"/>
-        <v>1358.7100000000009</v>
-      </c>
-      <c r="K42" s="3">
-        <f t="shared" si="5"/>
-        <v>1990.4900000000009</v>
-      </c>
-      <c r="L42" s="3">
-        <f t="shared" si="5"/>
-        <v>2953.4800000000005</v>
-      </c>
-      <c r="M42" s="3">
-        <f t="shared" si="5"/>
-        <v>3916.4700000000003</v>
-      </c>
-      <c r="N42" s="3">
-        <f t="shared" si="5"/>
-        <v>4879.46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="D43" s="3">
+        <v>1700</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1700</v>
+      </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -1692,20 +1646,19 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="P43" s="4">
-        <f>P37+P11</f>
+      <c r="O43" s="4">
+        <f>O37+O11</f>
         <v>21311.95</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3">
+        <v>34</v>
+      </c>
+      <c r="C44" s="3">
         <v>200</v>
       </c>
+      <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -1715,307 +1668,295 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3">
+        <v>35</v>
+      </c>
+      <c r="C45" s="3">
         <v>3286.89</v>
       </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3">
-        <v>3000</v>
-      </c>
+      <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3">
+      <c r="M45" s="3">
         <v>2800</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" ref="C47:M47" si="4">SUM(C41:C45)</f>
+        <v>5793.17</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="4"/>
+        <v>4309.7449999999999</v>
+      </c>
+      <c r="E47" s="7">
+        <f t="shared" si="4"/>
+        <v>4964.45</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="4"/>
+        <v>4230.84</v>
+      </c>
+      <c r="G47" s="7">
+        <f t="shared" si="4"/>
+        <v>4025.2700000000004</v>
+      </c>
+      <c r="H47" s="7">
+        <f t="shared" si="4"/>
+        <v>4034.4900000000007</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="4"/>
+        <v>4043.7100000000009</v>
+      </c>
+      <c r="J47" s="7">
+        <f t="shared" si="4"/>
+        <v>4675.4900000000007</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="4"/>
+        <v>5638.4800000000005</v>
+      </c>
+      <c r="L47" s="7">
+        <f t="shared" si="4"/>
+        <v>6601.47</v>
+      </c>
+      <c r="M47" s="7">
+        <f t="shared" si="4"/>
+        <v>10364.459999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="7">
-        <f t="shared" ref="C47:N47" si="6">SUM(C41:C45)</f>
-        <v>0</v>
-      </c>
-      <c r="D47" s="7">
+      <c r="C49" s="5">
+        <f t="shared" ref="C49:M49" si="5">C47-C39</f>
+        <v>309.74499999999989</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" si="5"/>
+        <v>964.44999999999982</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" si="5"/>
+        <v>1930.8400000000001</v>
+      </c>
+      <c r="F49" s="5">
+        <f t="shared" si="5"/>
+        <v>1725.2700000000004</v>
+      </c>
+      <c r="G49" s="5">
+        <f t="shared" si="5"/>
+        <v>1734.4900000000007</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" si="5"/>
+        <v>1743.7100000000009</v>
+      </c>
+      <c r="I49" s="5">
+        <f t="shared" si="5"/>
+        <v>2375.4900000000007</v>
+      </c>
+      <c r="J49" s="5">
+        <f t="shared" si="5"/>
+        <v>3338.4800000000005</v>
+      </c>
+      <c r="K49" s="5">
+        <f t="shared" si="5"/>
+        <v>4301.47</v>
+      </c>
+      <c r="L49" s="5">
+        <f t="shared" si="5"/>
+        <v>5264.46</v>
+      </c>
+      <c r="M49" s="5">
+        <f t="shared" si="5"/>
+        <v>9027.4499999999989</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="3">
+        <v>577.20000000000005</v>
+      </c>
+      <c r="E53" s="3">
+        <v>828</v>
+      </c>
+      <c r="F53" s="3">
+        <v>257</v>
+      </c>
+      <c r="G53" s="3">
+        <v>200</v>
+      </c>
+      <c r="H53" s="3">
+        <f>SUM(D53:G53)</f>
+        <v>1862.2</v>
+      </c>
+      <c r="I53" s="3"/>
+      <c r="K53" s="3">
+        <v>275</v>
+      </c>
+      <c r="M53" s="5">
+        <f>SUM(H53:K53)</f>
+        <v>2137.1999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3">
+        <v>828</v>
+      </c>
+      <c r="F54" s="3">
+        <v>257</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3">
+        <f t="shared" ref="H54:H58" si="6">SUM(D54:G54)</f>
+        <v>1085</v>
+      </c>
+      <c r="K54" s="3">
+        <v>275</v>
+      </c>
+      <c r="M54" s="5">
+        <f t="shared" ref="M54:M58" si="7">SUM(H54:K54)</f>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3">
+        <v>257</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3">
         <f t="shared" si="6"/>
-        <v>5793.17</v>
-      </c>
-      <c r="E47" s="7">
+        <v>257</v>
+      </c>
+      <c r="K55" s="3">
+        <v>275</v>
+      </c>
+      <c r="M55" s="5">
+        <f t="shared" si="7"/>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3">
+        <v>257</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3">
         <f t="shared" si="6"/>
-        <v>2624.7449999999999</v>
-      </c>
-      <c r="F47" s="7">
+        <v>257</v>
+      </c>
+      <c r="K56" s="3">
+        <v>275</v>
+      </c>
+      <c r="M56" s="5">
+        <f t="shared" si="7"/>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3">
+        <v>257</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3">
         <f t="shared" si="6"/>
-        <v>4579.45</v>
-      </c>
-      <c r="G47" s="7">
+        <v>257</v>
+      </c>
+      <c r="M57" s="5">
+        <f t="shared" si="7"/>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3">
+        <v>257</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3">
         <f t="shared" si="6"/>
-        <v>3845.84</v>
-      </c>
-      <c r="H47" s="7">
-        <f t="shared" si="6"/>
-        <v>3640.2700000000004</v>
-      </c>
-      <c r="I47" s="7">
-        <f t="shared" si="6"/>
-        <v>3649.4900000000007</v>
-      </c>
-      <c r="J47" s="7">
-        <f t="shared" si="6"/>
-        <v>3658.7100000000009</v>
-      </c>
-      <c r="K47" s="7">
-        <f t="shared" si="6"/>
-        <v>4290.4900000000007</v>
-      </c>
-      <c r="L47" s="7">
-        <f t="shared" si="6"/>
-        <v>5253.4800000000005</v>
-      </c>
-      <c r="M47" s="7">
-        <f t="shared" si="6"/>
-        <v>6216.47</v>
-      </c>
-      <c r="N47" s="7">
-        <f t="shared" si="6"/>
-        <v>9979.4599999999991</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="5">
-        <f t="shared" ref="C49:N49" si="7">C47-C39</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="5">
+        <v>257</v>
+      </c>
+      <c r="M58" s="5">
         <f t="shared" si="7"/>
-        <v>324.74499999999989</v>
-      </c>
-      <c r="E49" s="5">
-        <f t="shared" si="7"/>
-        <v>-720.55000000000018</v>
-      </c>
-      <c r="F49" s="5">
-        <f t="shared" si="7"/>
-        <v>1545.8400000000001</v>
-      </c>
-      <c r="G49" s="5">
-        <f t="shared" si="7"/>
-        <v>1340.2700000000004</v>
-      </c>
-      <c r="H49" s="5">
-        <f t="shared" si="7"/>
-        <v>1349.4900000000007</v>
-      </c>
-      <c r="I49" s="5">
-        <f t="shared" si="7"/>
-        <v>1358.7100000000009</v>
-      </c>
-      <c r="J49" s="5">
-        <f t="shared" si="7"/>
-        <v>1990.4900000000009</v>
-      </c>
-      <c r="K49" s="5">
-        <f t="shared" si="7"/>
-        <v>2953.4800000000005</v>
-      </c>
-      <c r="L49" s="5">
-        <f t="shared" si="7"/>
-        <v>3916.4700000000003</v>
-      </c>
-      <c r="M49" s="5">
-        <f t="shared" si="7"/>
-        <v>4879.46</v>
-      </c>
-      <c r="N49" s="5">
-        <f t="shared" si="7"/>
-        <v>8642.4499999999989</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E52" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E53" s="3">
-        <v>577.20000000000005</v>
-      </c>
-      <c r="F53" s="3">
-        <v>828</v>
-      </c>
-      <c r="G53" s="3">
         <v>257</v>
       </c>
-      <c r="H53" s="3">
-        <v>200</v>
-      </c>
-      <c r="I53" s="3">
-        <f>SUM(E53:H53)</f>
-        <v>1862.2</v>
-      </c>
-      <c r="J53" s="3"/>
-      <c r="L53" s="3">
-        <v>275</v>
-      </c>
-      <c r="N53" s="5">
-        <f>SUM(I53:L53)</f>
-        <v>2137.1999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3">
-        <v>828</v>
-      </c>
-      <c r="G54" s="3">
-        <v>257</v>
-      </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3">
-        <f t="shared" ref="I54:I58" si="8">SUM(E54:H54)</f>
-        <v>1085</v>
-      </c>
-      <c r="L54" s="3">
-        <v>275</v>
-      </c>
-      <c r="N54" s="5">
-        <f t="shared" ref="N54:N58" si="9">SUM(I54:L54)</f>
-        <v>1360</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D55" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3">
-        <v>257</v>
-      </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="L55" s="3">
-        <v>275</v>
-      </c>
-      <c r="N55" s="5">
-        <f t="shared" si="9"/>
-        <v>532</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3">
-        <v>257</v>
-      </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="L56" s="3">
-        <v>275</v>
-      </c>
-      <c r="N56" s="5">
-        <f t="shared" si="9"/>
-        <v>532</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D57" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3">
-        <v>257</v>
-      </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="N57" s="5">
-        <f t="shared" si="9"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D58" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3">
-        <v>257</v>
-      </c>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3">
-        <f t="shared" si="8"/>
-        <v>257</v>
-      </c>
-      <c r="N58" s="5">
-        <f t="shared" si="9"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="L59" s="4"/>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L60" s="4"/>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L61" s="4"/>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L62" s="4"/>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="4"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="4"/>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="4"/>
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K60" s="4"/>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K61" s="4"/>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K62" s="4"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="4"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="4"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>